<commit_message>
atualiza paper in press
</commit_message>
<xml_diff>
--- a/cv_data.xlsx
+++ b/cv_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="experience" sheetId="1" state="visible" r:id="rId2"/>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">Brasil</t>
   </si>
   <si>
-    <t xml:space="preserve">Evento ocorrido durante a \\href{sncticet.ufam.edu.br}{XV Semana Nacional de Ciência e Tecnologia de Itacoatiara (SNCT-ITA)};Duração de quatro horas, divididas em dois dias, duas horas cada; Este minicurso teve a intenção de abordar simplificadamente a produção de mapas de distribuição de espécies utilizando a linguagem R</t>
+    <t xml:space="preserve">Evento ocorrido durante a \href{https://www.sncticet.ufam.edu.br}{XV Semana Nacional de Ciência e Tecnologia de Itacoatiara (SNCT-ITA)};Duração de quatro horas, divididas em dois dias, duas horas cada; Este minicurso teve a intenção de abordar simplificadamente a produção de mapas de distribuição de espécies utilizando a linguagem R</t>
   </si>
   <si>
     <t xml:space="preserve">teaching</t>
@@ -120,7 +120,34 @@
     <t xml:space="preserve">Monitor da disciplina BOT-89 \textit{Preparação de dados para análise estatística  e Introdução ao uso de linguagem R}</t>
   </si>
   <si>
-    <t xml:space="preserve">Professor: Dr. Alberto Vicentini (INPA);Atuei como monitor por dois anos consecutivos;Criei um \\href{botanicaamazonica.wiki.br/labotam/doku.php?id=disciplinas:bot89:inicio}{sítio web} para auxiliar os discentes no aprendizado da disciplina</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Professor: Dr. Alberto Vicentini (INPA);Atuei como monitor por dois anos consecutivos;Criei um \href{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://www.botanicaamazonica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.wiki.br/labotam/doku.php?id=disciplinas:bot89:inicio}{sítio web} para auxiliar os discentes no aprendizado da disciplina</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">9--13 Nov 2015</t>
@@ -132,7 +159,7 @@
     <t xml:space="preserve">Programa de Pós-graduação em Recursos Naturais, UFRR</t>
   </si>
   <si>
-    <t xml:space="preserve">Professores: Dr. Reinaldo Imbrozio Barbosa (INPA), Lidiany Carvalho (UFRR);Auxiliei discentes em lidar com o ambiente R;Contribuí ativamente para o ensino do curso através de reuniões com o professor;Criei um \\href{http://www.botanicaamazonica.wiki.br/labotam/doku.php?id=alunos:r.perdiz:disciplina:inicio}{sítio web} para auxiliar os discentes no aprendizado do R</t>
+    <t xml:space="preserve">Professores: Dr. Reinaldo Imbrozio Barbosa (INPA), Lidiany Carvalho (UFRR);Auxiliei discentes em lidar com o ambiente R;Contribuí ativamente para o ensino do curso através de reuniões com o professor;Criei um \href{http://www.botanicaamazonica.wiki.br/labotam/doku.php?id=alunos:r.perdiz:disciplina:inicio}{sítio web} para auxiliar os discentes no aprendizado do R</t>
   </si>
   <si>
     <t xml:space="preserve">8--16 Ago 2013</t>
@@ -156,7 +183,7 @@
     <t xml:space="preserve">Brazil</t>
   </si>
   <si>
-    <t xml:space="preserve">Event that took place during the \\href{sncticet.ufam.edu.br}{XV Semana Nacional de Ciência e Tecnologia de Itacoatiara (SNCT-ITA)};Duration of four hours, divided into two days, two hours each;This short course had the intention of teaching in a simplified way how to produce species distribution maps using the R language</t>
+    <t xml:space="preserve">Event that took place during the \href{https://www.sncticet.ufam.edu.br}{XV Semana Nacional de Ciência e Tecnologia de Itacoatiara (SNCT-ITA)};Duration of four hours, divided into two days, two hours each;This short course had the intention of teaching in a simplified way how to produce species distribution maps using the R language</t>
   </si>
   <si>
     <t xml:space="preserve">english</t>
@@ -189,13 +216,13 @@
     <t xml:space="preserve">Graduate teaching assistant in BOT-89 \textit{Preparação de dados para análise estatística  e Introdução ao uso de linguagem R}</t>
   </si>
   <si>
-    <t xml:space="preserve">Teacher: Dr. Alberto Vicentini (INPA);Check the \\href{http://www.botanicaamazonica.wiki.br/labotam/doku.php?id=disciplinas:bot89:inicio}{website}</t>
+    <t xml:space="preserve">Teacher: Dr. Alberto Vicentini (INPA);Check the \href{http://www.botanicaamazonica.wiki.br/labotam/doku.php?id=disciplinas:bot89:inicio}{website}</t>
   </si>
   <si>
     <t xml:space="preserve">Graduate teaching assistant in PRN 235 \textit{Preparação de dados para análise estatística}</t>
   </si>
   <si>
-    <t xml:space="preserve">Teacher: Dr. Reinaldo Imbrozio Barbosa (INPA), Lidiany Carvalho (UFRR);Assisted students in dealing with R environment;Actively contributed to lecture course design through meetings with instructor;Created a \\href{botanicaamazonica.wiki.br/labotam/doku.php?id=alunos:r.perdiz:disciplina:inicio}{website} to help students in learning R</t>
+    <t xml:space="preserve">Teacher: Dr. Reinaldo Imbrozio Barbosa (INPA), Lidiany Carvalho (UFRR);Assisted students in dealing with R environment;Actively contributed to lecture course design through meetings with instructor;Created a \href{http://www.botanicaamazonica.wiki.br/labotam/doku.php?id=alunos:r.perdiz:disciplina:inicio}{website} to help students in learning R</t>
   </si>
   <si>
     <t xml:space="preserve">8--16 Aug 2013</t>
@@ -322,7 +349,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -343,6 +370,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -419,17 +453,17 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F9" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="96.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="75.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="56.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="62.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,6 +902,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" display="http://www.botanicaamazonica"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -889,9 +926,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,11 +1110,11 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">

</xml_diff>